<commit_message>
Final validation with groundtruth
</commit_message>
<xml_diff>
--- a/evalutation/eval.xlsx
+++ b/evalutation/eval.xlsx
@@ -502,37 +502,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.07012338468422917</v>
+        <v>0.06464670093312194</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8327380952380953</v>
+        <v>0.5485930735930735</v>
       </c>
       <c r="D2" t="n">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="E2" t="n">
-        <v>0.67</v>
+        <v>0.36</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7235347808525254</v>
+        <v>0.4112690190658179</v>
       </c>
       <c r="G2" t="n">
-        <v>0.95</v>
+        <v>0.7</v>
       </c>
       <c r="H2" t="n">
-        <v>0.58</v>
+        <v>0.295</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7212477028192306</v>
+        <v>0.4444382947895094</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K2" t="n">
-        <v>0.525</v>
+        <v>0.26</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8404314552702706</v>
+        <v>0.5776830350197704</v>
       </c>
     </row>
     <row r="3">
@@ -542,37 +542,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06690931866867381</v>
+        <v>0.1032633878887499</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8538461538461538</v>
+        <v>0.6445833333333333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="E3" t="n">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7041584385157289</v>
+        <v>0.4934383013479232</v>
       </c>
       <c r="G3" t="n">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5700000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6977722754739762</v>
+        <v>0.5337524086809473</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5425</v>
+        <v>0.3325</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8268170689390004</v>
+        <v>0.6548962121472878</v>
       </c>
     </row>
     <row r="4">
@@ -582,37 +582,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01799111577796716</v>
+        <v>0.01217881055873414</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4887121212121212</v>
+        <v>0.2508333333333334</v>
       </c>
       <c r="D4" t="n">
-        <v>0.55</v>
+        <v>0.35</v>
       </c>
       <c r="E4" t="n">
-        <v>0.29</v>
+        <v>0.12</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3359774193369671</v>
+        <v>0.1993788955987748</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="H4" t="n">
-        <v>0.265</v>
+        <v>0.095</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3762437560857868</v>
+        <v>0.2504468758412321</v>
       </c>
       <c r="J4" t="n">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="K4" t="n">
-        <v>0.27</v>
+        <v>0.065</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5554976105575509</v>
+        <v>0.2856531668212503</v>
       </c>
     </row>
     <row r="5">
@@ -622,37 +622,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.003169833559684963</v>
+        <v>0.0007913807527656885</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1516666666666667</v>
+        <v>0.02083333333333333</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="E5" t="n">
-        <v>0.12</v>
+        <v>0.01</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1312827986181829</v>
+        <v>0.01173196815056891</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="H5" t="n">
-        <v>0.125</v>
+        <v>0.005</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1725027502266829</v>
+        <v>0.01173196815056891</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1025</v>
+        <v>0.01</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1963012760954803</v>
+        <v>0.03693028757952595</v>
       </c>
     </row>
     <row r="6">
@@ -662,37 +662,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01876180673292137</v>
+        <v>0.02648119535087895</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6041666666666667</v>
+        <v>0.3866666666666667</v>
       </c>
       <c r="D6" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4400000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5046749077630367</v>
+        <v>0.331422143515167</v>
       </c>
       <c r="G6" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="H6" t="n">
-        <v>0.395</v>
+        <v>0.15</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5208279167156444</v>
+        <v>0.379808336442854</v>
       </c>
       <c r="J6" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K6" t="n">
-        <v>0.38</v>
+        <v>0.135</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6132586067289071</v>
+        <v>0.4652837515752271</v>
       </c>
     </row>
     <row r="7">
@@ -702,37 +702,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0425686424020103</v>
+        <v>0.06306760132418662</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6397222222222222</v>
+        <v>0.4191883116883117</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.52</v>
+        <v>0.24</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5531443003033248</v>
+        <v>0.3019956889389471</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H7" t="n">
-        <v>0.475</v>
+        <v>0.26</v>
       </c>
       <c r="I7" t="n">
-        <v>0.592026027182087</v>
+        <v>0.4049221295690922</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4725</v>
+        <v>0.225</v>
       </c>
       <c r="L7" t="n">
-        <v>0.745432566077509</v>
+        <v>0.5153684564058171</v>
       </c>
     </row>
     <row r="8">
@@ -742,37 +742,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08039377089263025</v>
+        <v>0.08009889375229304</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7816666666666666</v>
+        <v>0.6273856209150327</v>
       </c>
       <c r="D8" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.4632436778799587</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.4946707556277395</v>
+      </c>
+      <c r="J8" t="n">
         <v>0.95</v>
       </c>
-      <c r="E8" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.704688179629027</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.7321848289765063</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
       <c r="K8" t="n">
-        <v>0.58</v>
+        <v>0.29</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8438279235505426</v>
+        <v>0.6545760439140381</v>
       </c>
     </row>
     <row r="9">
@@ -782,37 +782,37 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1000248360392397</v>
+        <v>0.1333599610344434</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8458333333333334</v>
+        <v>0.6330555555555556</v>
       </c>
       <c r="D9" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.5371131665741533</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.95</v>
       </c>
-      <c r="E9" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.780760830181962</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
       <c r="H9" t="n">
-        <v>0.73</v>
+        <v>0.48</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7792865778632365</v>
+        <v>0.6088651634217641</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7</v>
+        <v>0.375</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8818784314280503</v>
+        <v>0.705027786819972</v>
       </c>
     </row>
     <row r="10">
@@ -822,37 +822,37 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.05317183117368644</v>
+        <v>0.07408224170163608</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7479166666666667</v>
+        <v>0.5176190476190476</v>
       </c>
       <c r="D10" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.4194558842742613</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.4512070000682071</v>
+      </c>
+      <c r="J10" t="n">
         <v>0.9</v>
       </c>
-      <c r="E10" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.5861503824332088</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.515</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.6230629111390253</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
       <c r="K10" t="n">
-        <v>0.475</v>
+        <v>0.26</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7715656920957823</v>
+        <v>0.5902754080035516</v>
       </c>
     </row>
     <row r="11">
@@ -862,37 +862,37 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.08122162497840565</v>
+        <v>0.1413495868258528</v>
       </c>
       <c r="C11" t="n">
-        <v>0.89375</v>
+        <v>0.6338095238095238</v>
       </c>
       <c r="D11" t="n">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="E11" t="n">
-        <v>0.77</v>
+        <v>0.52</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8263199280384239</v>
+        <v>0.5356246564120216</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="H11" t="n">
-        <v>0.65</v>
+        <v>0.46</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7808266196881385</v>
+        <v>0.5968113702335774</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="K11" t="n">
-        <v>0.5974999999999999</v>
+        <v>0.365</v>
       </c>
       <c r="L11" t="n">
-        <v>0.8777262141690902</v>
+        <v>0.6946581110815202</v>
       </c>
     </row>
     <row r="12">
@@ -902,37 +902,37 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03402599846906525</v>
+        <v>0.04780561722605171</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5562103174603175</v>
+        <v>0.3492507002801121</v>
       </c>
       <c r="D12" t="n">
-        <v>0.65</v>
+        <v>0.55</v>
       </c>
       <c r="E12" t="n">
-        <v>0.36</v>
+        <v>0.21</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4326774004224713</v>
+        <v>0.2551363016939682</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="H12" t="n">
-        <v>0.355</v>
+        <v>0.225</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5085822472920357</v>
+        <v>0.3377482070611812</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3425</v>
+        <v>0.205</v>
       </c>
       <c r="L12" t="n">
-        <v>0.6153889382100279</v>
+        <v>0.4544895806975411</v>
       </c>
     </row>
     <row r="13">
@@ -942,37 +942,37 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.04481990948552043</v>
+        <v>0.07670534755380193</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5739583333333333</v>
+        <v>0.440021645021645</v>
       </c>
       <c r="D13" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3624276790413858</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.7</v>
       </c>
-      <c r="E13" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.493886904165764</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.8</v>
-      </c>
       <c r="H13" t="n">
-        <v>0.4349999999999999</v>
+        <v>0.28</v>
       </c>
       <c r="I13" t="n">
-        <v>0.526311806232428</v>
+        <v>0.402292193973452</v>
       </c>
       <c r="J13" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4075</v>
+        <v>0.255</v>
       </c>
       <c r="L13" t="n">
-        <v>0.6365173396653351</v>
+        <v>0.5390832808130274</v>
       </c>
     </row>
     <row r="14">
@@ -982,37 +982,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.07322073597037332</v>
+        <v>0.08679691399624502</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8433333333333334</v>
+        <v>0.5867857142857142</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E14" t="n">
-        <v>0.74</v>
+        <v>0.4400000000000001</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7505201382919194</v>
+        <v>0.5048487178884085</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H14" t="n">
-        <v>0.6599999999999999</v>
+        <v>0.39</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7686489666445397</v>
+        <v>0.5896595202628588</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="K14" t="n">
-        <v>0.5650000000000001</v>
+        <v>0.275</v>
       </c>
       <c r="L14" t="n">
-        <v>0.8632852383042948</v>
+        <v>0.6773282210144329</v>
       </c>
     </row>
     <row r="15">
@@ -1022,37 +1022,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.1000248360392397</v>
+        <v>0.1366038510539645</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8458333333333334</v>
+        <v>0.5946078431372549</v>
       </c>
       <c r="D15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.4622699507445558</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.95</v>
       </c>
-      <c r="E15" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.780760830181962</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
       <c r="H15" t="n">
-        <v>0.73</v>
+        <v>0.42</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7792865778632365</v>
+        <v>0.5216825716850432</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0.7</v>
+        <v>0.38</v>
       </c>
       <c r="L15" t="n">
-        <v>0.8818784314280503</v>
+        <v>0.6880541590235631</v>
       </c>
     </row>
     <row r="16">
@@ -1062,37 +1062,37 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01109853640048079</v>
+        <v>0.0007410862354892205</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5953044871794873</v>
+        <v>0.01041666666666667</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.4639458380888314</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
       <c r="H16" t="n">
-        <v>0.295</v>
+        <v>0.005</v>
       </c>
       <c r="I16" t="n">
-        <v>0.4809727639454702</v>
+        <v>0.01577324383928644</v>
       </c>
       <c r="J16" t="n">
-        <v>0.85</v>
+        <v>0.1</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2725</v>
+        <v>0.005</v>
       </c>
       <c r="L16" t="n">
-        <v>0.6098285376425937</v>
+        <v>0.02928515156065242</v>
       </c>
     </row>
     <row r="17">
@@ -1102,37 +1102,37 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0005701277042907878</v>
+        <v>0.001242507213095448</v>
       </c>
       <c r="C17" t="n">
-        <v>0.07417515082956258</v>
+        <v>0.01571895424836601</v>
       </c>
       <c r="D17" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.01185988563846481</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.02278025747937302</v>
+      </c>
+      <c r="J17" t="n">
         <v>0.15</v>
       </c>
-      <c r="E17" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.05485761194248029</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.0891790883536238</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.45</v>
-      </c>
       <c r="K17" t="n">
-        <v>0.0525</v>
+        <v>0.01</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1729681840886544</v>
+        <v>0.0465413264761115</v>
       </c>
     </row>
     <row r="18">
@@ -1142,37 +1142,37 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01838596976824773</v>
+        <v>0.03033487295889143</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5199548112706007</v>
+        <v>0.3460598633392751</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="E18" t="n">
-        <v>0.42</v>
+        <v>0.15</v>
       </c>
       <c r="F18" t="n">
-        <v>0.4720668947643206</v>
+        <v>0.2347952947152387</v>
       </c>
       <c r="G18" t="n">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
       <c r="H18" t="n">
-        <v>0.4</v>
+        <v>0.17</v>
       </c>
       <c r="I18" t="n">
-        <v>0.534192736273253</v>
+        <v>0.3322877937678121</v>
       </c>
       <c r="J18" t="n">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="K18" t="n">
-        <v>0.38</v>
+        <v>0.15</v>
       </c>
       <c r="L18" t="n">
-        <v>0.6489211635233378</v>
+        <v>0.4399001810619153</v>
       </c>
     </row>
     <row r="19">
@@ -1182,37 +1182,37 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.001011756516688751</v>
+        <v>0.0007997332125239103</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0904532967032967</v>
+        <v>0.01964285714285714</v>
       </c>
       <c r="D19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.01320340612862954</v>
+      </c>
+      <c r="G19" t="n">
         <v>0.1</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.03666734242976737</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.25</v>
-      </c>
       <c r="H19" t="n">
-        <v>0.035</v>
+        <v>0.01</v>
       </c>
       <c r="I19" t="n">
-        <v>0.08378072884548585</v>
+        <v>0.02987007279529621</v>
       </c>
       <c r="J19" t="n">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="K19" t="n">
-        <v>0.04</v>
+        <v>0.007500000000000001</v>
       </c>
       <c r="L19" t="n">
-        <v>0.1463321842943786</v>
+        <v>0.03842172699868211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>